<commit_message>
return product flow add
</commit_message>
<xml_diff>
--- a/tzc_sales_customization_spt/sample/Case Report.xlsx
+++ b/tzc_sales_customization_spt/sample/Case Report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Billing Address:</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t xml:space="preserve">Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case Type</t>
   </si>
   <si>
     <t xml:space="preserve">Category</t>
@@ -197,15 +200,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,6 +314,9 @@
       </c>
       <c r="G14" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>